<commit_message>
add vega popup for CH
</commit_message>
<xml_diff>
--- a/data/Travel History.xlsx
+++ b/data/Travel History.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lwyoh\myflightlog\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0416C39D-DE4F-4744-BA1A-1AF76865C405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC534F46-7B6E-4166-B8B4-22BE6799A86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19298" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="93">
   <si>
     <t>Country</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Valais</t>
   </si>
   <si>
-    <t>Lucerne</t>
-  </si>
-  <si>
     <t>Schwyz</t>
   </si>
   <si>
@@ -213,9 +210,6 @@
     <t>2024-01</t>
   </si>
   <si>
-    <t>Geneva</t>
-  </si>
-  <si>
     <t>2023-08</t>
   </si>
   <si>
@@ -301,6 +295,15 @@
   </si>
   <si>
     <t>HKG</t>
+  </si>
+  <si>
+    <t>Fribourg</t>
+  </si>
+  <si>
+    <t>Luzern</t>
+  </si>
+  <si>
+    <t>Genève</t>
   </si>
 </sst>
 </file>
@@ -624,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,10 +644,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -655,13 +658,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -669,13 +672,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -683,13 +686,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -697,13 +700,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -711,13 +714,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -725,13 +728,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -739,13 +742,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -753,13 +756,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -767,13 +770,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -781,13 +784,13 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,13 +798,13 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -809,13 +812,13 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -823,13 +826,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -837,13 +840,13 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -851,13 +854,13 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -865,13 +868,13 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -879,13 +882,13 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -893,13 +896,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -907,13 +910,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -921,27 +924,27 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -949,13 +952,13 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -963,13 +966,13 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -977,13 +980,13 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -991,69 +994,69 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
       <c r="D27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="B28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
       <c r="D28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
         <v>33</v>
       </c>
-      <c r="B30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1061,97 +1064,97 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
         <v>38</v>
       </c>
-      <c r="B33" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" t="s">
-        <v>39</v>
-      </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1159,13 +1162,13 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1173,55 +1176,55 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
         <v>47</v>
       </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>48</v>
-      </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1229,27 +1232,41 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
         <v>51</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" t="s">
         <v>90</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D45" t="s">
         <v>52</v>
-      </c>
-      <c r="D44" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>